<commit_message>
Dashboard Cubo Compras completo
Eliminando mallado de excel
</commit_message>
<xml_diff>
--- a/BI_Proyecto.xlsx
+++ b/BI_Proyecto.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugoe\OneDrive\Documents\N-capas\Biblioteca\Proyecto_BI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0610D73D-4E43-497C-AE84-DAE38E6872CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C29842-C213-4097-A41F-C4B68AA0D48A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="855" yWindow="-120" windowWidth="19755" windowHeight="11760" xr2:uid="{7364818D-8A95-4AD3-8FD8-14EFEEC2FBFC}"/>
+    <workbookView xWindow="855" yWindow="-120" windowWidth="19755" windowHeight="11760" activeTab="1" xr2:uid="{7364818D-8A95-4AD3-8FD8-14EFEEC2FBFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,9 @@
   </sheets>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="122" r:id="rId3"/>
-    <pivotCache cacheId="142" r:id="rId4"/>
-    <pivotCache cacheId="151" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="2" r:id="rId4"/>
+    <pivotCache cacheId="8" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -542,49 +542,7 @@
           </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -616,7 +574,6 @@
               <a:endParaRPr lang="es-SV"/>
             </a:p>
           </c:txPr>
-          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -961,7 +918,7 @@
                 <c:formatCode>"$"#,##0.00</c:formatCode>
                 <c:ptCount val="86"/>
                 <c:pt idx="0">
-                  <c:v>28502.091799999998</c:v>
+                  <c:v>28502.091800000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>498589.59150000004</c:v>
@@ -976,19 +933,19 @@
                   <c:v>824365.1679</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30229.374800000005</c:v>
+                  <c:v>30229.374800000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25060.0429</c:v>
+                  <c:v>25060.042899999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79384.768000000011</c:v>
+                  <c:v>79384.767999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>38622.123899999991</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1952375.2986000001</c:v>
+                  <c:v>1952375.2985999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>87404.101300000009</c:v>
@@ -1000,13 +957,13 @@
                   <c:v>5779.9932000000008</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8497.798499999999</c:v>
+                  <c:v>8497.7985000000008</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>770340.44460000005</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>561550.09519999987</c:v>
+                  <c:v>561550.09519999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>3347165.1964999996</c:v>
@@ -1015,7 +972,7 @@
                   <c:v>31101.197399999997</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>324301.47960000002</c:v>
+                  <c:v>324301.47959999996</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>1582013.0589000001</c:v>
@@ -1030,34 +987,34 @@
                   <c:v>1594705.6125</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3378.1736999999989</c:v>
+                  <c:v>3378.1736999999998</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>22960.072400000005</c:v>
+                  <c:v>22960.072399999997</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2472770.0523000006</c:v>
+                  <c:v>2472770.0523000001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>31499.814100000003</c:v>
+                  <c:v>31499.814099999996</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1315488.5502000002</c:v>
+                  <c:v>1315488.5501999999</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2154773.3718000003</c:v>
+                  <c:v>2154773.3717999998</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>1145708.7844000002</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>71924.478900000016</c:v>
+                  <c:v>71924.478900000002</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>112931.19209999999</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2304231.5536000002</c:v>
+                  <c:v>2304231.5535999998</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>609422</c:v>
@@ -1066,40 +1023,40 @@
                   <c:v>5036.1464999999998</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>25633.635299999998</c:v>
+                  <c:v>25633.635300000002</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>76348.25</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2472770.0523000006</c:v>
+                  <c:v>2472770.0523000001</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>401930.90310000005</c:v>
+                  <c:v>401930.9031</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>1597309.2135000001</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1268930.0360999997</c:v>
+                  <c:v>1268930.0360999999</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1952375.2985999994</c:v>
+                  <c:v>1952375.2985999999</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>27308.607400000004</c:v>
+                  <c:v>27308.607400000001</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>1186835.76</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>8061.1008000000002</c:v>
+                  <c:v>8061.1007999999993</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1589172.9591000003</c:v>
+                  <c:v>1589172.9591000001</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>209264.42909999998</c:v>
+                  <c:v>209264.42910000001</c:v>
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>24070.75</c:v>
@@ -1111,13 +1068,13 @@
                   <c:v>42658</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>321870.17490000004</c:v>
+                  <c:v>321870.17489999998</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>27177.800499999998</c:v>
+                  <c:v>27177.800500000001</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>5412.5649999999987</c:v>
+                  <c:v>5412.5649999999996</c:v>
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>8553.3241999999991</c:v>
@@ -1126,19 +1083,19 @@
                   <c:v>6324.5249999999996</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>7328.72</c:v>
+                  <c:v>7328.7199999999993</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2424284.3650000002</c:v>
+                  <c:v>2424284.3649999998</c:v>
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>23146.99</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>39754.446499999991</c:v>
+                  <c:v>39754.446499999998</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>25513.899999999998</c:v>
+                  <c:v>25513.899999999994</c:v>
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>31824.150099999999</c:v>
@@ -1153,13 +1110,13 @@
                   <c:v>28220.146600000004</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>3379946.3215000005</c:v>
+                  <c:v>3379946.3215000001</c:v>
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>2593901.3108999999</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>23635.058400000005</c:v>
+                  <c:v>23635.058400000002</c:v>
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>26100.821099999997</c:v>
@@ -1171,7 +1128,7 @@
                   <c:v>25732.837800000001</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>2675889.2159999991</c:v>
+                  <c:v>2675889.2159999995</c:v>
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>328640.815</c:v>
@@ -1186,22 +1143,22 @@
                   <c:v>436401.9</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>91088.374599999996</c:v>
+                  <c:v>91088.37460000001</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>577793.36319999991</c:v>
+                  <c:v>577793.36320000002</c:v>
                 </c:pt>
                 <c:pt idx="77">
                   <c:v>1461653.9449999998</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>52176.445000000007</c:v>
+                  <c:v>52176.445</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>2052173.6244000001</c:v>
+                  <c:v>2052173.6244000003</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>2777684.9109999998</c:v>
+                  <c:v>2777684.9110000003</c:v>
                 </c:pt>
                 <c:pt idx="81">
                   <c:v>2090857.52</c:v>
@@ -1213,7 +1170,7 @@
                   <c:v>25060.0429</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>8025.5997000000007</c:v>
+                  <c:v>8025.5996999999988</c:v>
                 </c:pt>
                 <c:pt idx="85">
                   <c:v>6947.5750000000007</c:v>
@@ -1228,7 +1185,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1588,8 +1544,7 @@
           </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -1632,6 +1587,211 @@
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
@@ -1693,6 +1853,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-66D9-4147-9475-B5025818527D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1735,6 +1900,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-66D9-4147-9475-B5025818527D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1777,6 +1947,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-66D9-4147-9475-B5025818527D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1819,6 +1994,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-66D9-4147-9475-B5025818527D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -1861,6 +2041,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-66D9-4147-9475-B5025818527D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -2218,8 +2403,7 @@
           </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -2262,6 +2446,88 @@
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
@@ -2323,6 +2589,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-0796-4D0B-BD92-575C60FB8981}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -2365,6 +2636,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-0796-4D0B-BD92-575C60FB8981}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -4361,7 +4637,122 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Hugo Doradea" refreshedDate="44373.092452893521" backgroundQuery="1" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{9375D43D-8078-4D86-801E-D223FAB557BC}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Hugo Doradea" refreshedDate="44373.098925578706" backgroundQuery="1" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{4EAE0EA9-E97F-4F06-8090-CC4A09B30996}">
+  <cacheSource type="external" connectionId="2"/>
+  <cacheFields count="2">
+    <cacheField name="[Measures].[Total Due]" caption="Total Due" numFmtId="0" hierarchy="9" level="32767"/>
+    <cacheField name="[dim_ship_method].[Jerarquía].[Name]" caption="Name" numFmtId="0" hierarchy="3" level="1">
+      <sharedItems count="5">
+        <s v="[dim_ship_method].[Jerarquía].[Name].&amp;[CARGO TRANSPORT 5]" c="CARGO TRANSPORT 5"/>
+        <s v="[dim_ship_method].[Jerarquía].[Name].&amp;[OVERNIGHT J-FAST]" c="OVERNIGHT J-FAST"/>
+        <s v="[dim_ship_method].[Jerarquía].[Name].&amp;[OVERSEAS - DELUXE]" c="OVERSEAS - DELUXE"/>
+        <s v="[dim_ship_method].[Jerarquía].[Name].&amp;[XRQ - TRUCK GROUND]" c="XRQ - TRUCK GROUND"/>
+        <s v="[dim_ship_method].[Jerarquía].[Name].&amp;[ZY - EXPRESS]" c="ZY - EXPRESS"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <cacheHierarchies count="10">
+    <cacheHierarchy uniqueName="[dim_employee].[Business Entity ID]" caption="Business Entity ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[dim_employee].[Business Entity ID].[All]" allUniqueName="[dim_employee].[Business Entity ID].[All]" dimensionUniqueName="[dim_employee]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[dim_employee].[Gender]" caption="Gender" attribute="1" defaultMemberUniqueName="[dim_employee].[Gender].[All]" allUniqueName="[dim_employee].[Gender].[All]" dimensionUniqueName="[dim_employee]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[dim_employee].[Jerarquía]" caption="Jerarquía" defaultMemberUniqueName="[dim_employee].[Jerarquía].[All]" allUniqueName="[dim_employee].[Jerarquía].[All]" dimensionUniqueName="[dim_employee]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[dim_ship_method].[Jerarquía]" caption="Jerarquía" defaultMemberUniqueName="[dim_ship_method].[Jerarquía].[All]" allUniqueName="[dim_ship_method].[Jerarquía].[All]" dimensionUniqueName="[dim_ship_method]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[dim_ship_method].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[dim_ship_method].[Name].[All]" allUniqueName="[dim_ship_method].[Name].[All]" dimensionUniqueName="[dim_ship_method]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[dim_ship_method].[Ship Method ID]" caption="Ship Method ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[dim_ship_method].[Ship Method ID].[All]" allUniqueName="[dim_ship_method].[Ship Method ID].[All]" dimensionUniqueName="[dim_ship_method]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[dim_vendor].[Business Entity ID]" caption="Business Entity ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[dim_vendor].[Business Entity ID].[All]" allUniqueName="[dim_vendor].[Business Entity ID].[All]" dimensionUniqueName="[dim_vendor]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[dim_vendor].[Jerarquía]" caption="Jerarquía" defaultMemberUniqueName="[dim_vendor].[Jerarquía].[All]" allUniqueName="[dim_vendor].[Jerarquía].[All]" dimensionUniqueName="[dim_vendor]" displayFolder="" count="2" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[dim_vendor].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[dim_vendor].[Name].[All]" allUniqueName="[dim_vendor].[Name].[All]" dimensionUniqueName="[dim_vendor]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Total Due]" caption="Total Due" measure="1" displayFolder="" measureGroup="Purchase Order Header" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <dimensions count="4">
+    <dimension name="dim_employee" uniqueName="[dim_employee]" caption="dim_employee"/>
+    <dimension name="dim_ship_method" uniqueName="[dim_ship_method]" caption="dim_ship_method"/>
+    <dimension name="dim_vendor" uniqueName="[dim_vendor]" caption="dim_vendor"/>
+    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
+  </dimensions>
+  <measureGroups count="1">
+    <measureGroup name="Purchase Order Header" caption="Purchase Order Header"/>
+  </measureGroups>
+  <maps count="3">
+    <map measureGroup="0" dimension="0"/>
+    <map measureGroup="0" dimension="1"/>
+    <map measureGroup="0" dimension="2"/>
+  </maps>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Hugo Doradea" refreshedDate="44373.099563425923" backgroundQuery="1" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{C61F9162-62DE-4C5C-AFA1-CA6D16A03B11}">
+  <cacheSource type="external" connectionId="2"/>
+  <cacheFields count="2">
+    <cacheField name="[Measures].[Total Due]" caption="Total Due" numFmtId="0" hierarchy="9" level="32767"/>
+    <cacheField name="[dim_employee].[Jerarquía].[Gender]" caption="Gender" numFmtId="0" hierarchy="2" level="1">
+      <sharedItems count="2">
+        <s v="[dim_employee].[Jerarquía].[Gender].&amp;[F]" c="F"/>
+        <s v="[dim_employee].[Jerarquía].[Gender].&amp;[M]" c="M"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <cacheHierarchies count="10">
+    <cacheHierarchy uniqueName="[dim_employee].[Business Entity ID]" caption="Business Entity ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[dim_employee].[Business Entity ID].[All]" allUniqueName="[dim_employee].[Business Entity ID].[All]" dimensionUniqueName="[dim_employee]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[dim_employee].[Gender]" caption="Gender" attribute="1" defaultMemberUniqueName="[dim_employee].[Gender].[All]" allUniqueName="[dim_employee].[Gender].[All]" dimensionUniqueName="[dim_employee]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[dim_employee].[Jerarquía]" caption="Jerarquía" defaultMemberUniqueName="[dim_employee].[Jerarquía].[All]" allUniqueName="[dim_employee].[Jerarquía].[All]" dimensionUniqueName="[dim_employee]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[dim_ship_method].[Jerarquía]" caption="Jerarquía" defaultMemberUniqueName="[dim_ship_method].[Jerarquía].[All]" allUniqueName="[dim_ship_method].[Jerarquía].[All]" dimensionUniqueName="[dim_ship_method]" displayFolder="" count="2" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[dim_ship_method].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[dim_ship_method].[Name].[All]" allUniqueName="[dim_ship_method].[Name].[All]" dimensionUniqueName="[dim_ship_method]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[dim_ship_method].[Ship Method ID]" caption="Ship Method ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[dim_ship_method].[Ship Method ID].[All]" allUniqueName="[dim_ship_method].[Ship Method ID].[All]" dimensionUniqueName="[dim_ship_method]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[dim_vendor].[Business Entity ID]" caption="Business Entity ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[dim_vendor].[Business Entity ID].[All]" allUniqueName="[dim_vendor].[Business Entity ID].[All]" dimensionUniqueName="[dim_vendor]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[dim_vendor].[Jerarquía]" caption="Jerarquía" defaultMemberUniqueName="[dim_vendor].[Jerarquía].[All]" allUniqueName="[dim_vendor].[Jerarquía].[All]" dimensionUniqueName="[dim_vendor]" displayFolder="" count="2" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[dim_vendor].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[dim_vendor].[Name].[All]" allUniqueName="[dim_vendor].[Name].[All]" dimensionUniqueName="[dim_vendor]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Total Due]" caption="Total Due" measure="1" displayFolder="" measureGroup="Purchase Order Header" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <dimensions count="4">
+    <dimension name="dim_employee" uniqueName="[dim_employee]" caption="dim_employee"/>
+    <dimension name="dim_ship_method" uniqueName="[dim_ship_method]" caption="dim_ship_method"/>
+    <dimension name="dim_vendor" uniqueName="[dim_vendor]" caption="dim_vendor"/>
+    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
+  </dimensions>
+  <measureGroups count="1">
+    <measureGroup name="Purchase Order Header" caption="Purchase Order Header"/>
+  </measureGroups>
+  <maps count="3">
+    <map measureGroup="0" dimension="0"/>
+    <map measureGroup="0" dimension="1"/>
+    <map measureGroup="0" dimension="2"/>
+  </maps>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Hugo Doradea" refreshedDate="44373.115628935186" backgroundQuery="1" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{9375D43D-8078-4D86-801E-D223FAB557BC}">
   <cacheSource type="external" connectionId="2"/>
   <cacheFields count="2">
     <cacheField name="[Measures].[Total Due]" caption="Total Due" numFmtId="0" hierarchy="9" level="32767"/>
@@ -4460,7 +4851,7 @@
     <cacheHierarchy uniqueName="[dim_employee].[Business Entity ID]" caption="Business Entity ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[dim_employee].[Business Entity ID].[All]" allUniqueName="[dim_employee].[Business Entity ID].[All]" dimensionUniqueName="[dim_employee]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[dim_employee].[Gender]" caption="Gender" attribute="1" defaultMemberUniqueName="[dim_employee].[Gender].[All]" allUniqueName="[dim_employee].[Gender].[All]" dimensionUniqueName="[dim_employee]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[dim_employee].[Jerarquía]" caption="Jerarquía" defaultMemberUniqueName="[dim_employee].[Jerarquía].[All]" allUniqueName="[dim_employee].[Jerarquía].[All]" dimensionUniqueName="[dim_employee]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[dim_ship_method].[Jerarquía]" caption="Jerarquía" defaultMemberUniqueName="[dim_ship_method].[Jerarquía].[All]" allUniqueName="[dim_ship_method].[Jerarquía].[All]" dimensionUniqueName="[dim_ship_method]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[dim_ship_method].[Jerarquía]" caption="Jerarquía" defaultMemberUniqueName="[dim_ship_method].[Jerarquía].[All]" allUniqueName="[dim_ship_method].[Jerarquía].[All]" dimensionUniqueName="[dim_ship_method]" displayFolder="" count="2" unbalanced="0"/>
     <cacheHierarchy uniqueName="[dim_ship_method].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[dim_ship_method].[Name].[All]" allUniqueName="[dim_ship_method].[Name].[All]" dimensionUniqueName="[dim_ship_method]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[dim_ship_method].[Ship Method ID]" caption="Ship Method ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[dim_ship_method].[Ship Method ID].[All]" allUniqueName="[dim_ship_method].[Ship Method ID].[All]" dimensionUniqueName="[dim_ship_method]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[dim_vendor].[Business Entity ID]" caption="Business Entity ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[dim_vendor].[Business Entity ID].[All]" allUniqueName="[dim_vendor].[Business Entity ID].[All]" dimensionUniqueName="[dim_vendor]" displayFolder="" count="0" unbalanced="0"/>
@@ -4500,123 +4891,8 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Hugo Doradea" refreshedDate="44373.098925578706" backgroundQuery="1" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{4EAE0EA9-E97F-4F06-8090-CC4A09B30996}">
-  <cacheSource type="external" connectionId="2"/>
-  <cacheFields count="2">
-    <cacheField name="[Measures].[Total Due]" caption="Total Due" numFmtId="0" hierarchy="9" level="32767"/>
-    <cacheField name="[dim_ship_method].[Jerarquía].[Name]" caption="Name" numFmtId="0" hierarchy="3" level="1">
-      <sharedItems count="5">
-        <s v="[dim_ship_method].[Jerarquía].[Name].&amp;[CARGO TRANSPORT 5]" c="CARGO TRANSPORT 5"/>
-        <s v="[dim_ship_method].[Jerarquía].[Name].&amp;[OVERNIGHT J-FAST]" c="OVERNIGHT J-FAST"/>
-        <s v="[dim_ship_method].[Jerarquía].[Name].&amp;[OVERSEAS - DELUXE]" c="OVERSEAS - DELUXE"/>
-        <s v="[dim_ship_method].[Jerarquía].[Name].&amp;[XRQ - TRUCK GROUND]" c="XRQ - TRUCK GROUND"/>
-        <s v="[dim_ship_method].[Jerarquía].[Name].&amp;[ZY - EXPRESS]" c="ZY - EXPRESS"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-  <cacheHierarchies count="10">
-    <cacheHierarchy uniqueName="[dim_employee].[Business Entity ID]" caption="Business Entity ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[dim_employee].[Business Entity ID].[All]" allUniqueName="[dim_employee].[Business Entity ID].[All]" dimensionUniqueName="[dim_employee]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[dim_employee].[Gender]" caption="Gender" attribute="1" defaultMemberUniqueName="[dim_employee].[Gender].[All]" allUniqueName="[dim_employee].[Gender].[All]" dimensionUniqueName="[dim_employee]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[dim_employee].[Jerarquía]" caption="Jerarquía" defaultMemberUniqueName="[dim_employee].[Jerarquía].[All]" allUniqueName="[dim_employee].[Jerarquía].[All]" dimensionUniqueName="[dim_employee]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[dim_ship_method].[Jerarquía]" caption="Jerarquía" defaultMemberUniqueName="[dim_ship_method].[Jerarquía].[All]" allUniqueName="[dim_ship_method].[Jerarquía].[All]" dimensionUniqueName="[dim_ship_method]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[dim_ship_method].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[dim_ship_method].[Name].[All]" allUniqueName="[dim_ship_method].[Name].[All]" dimensionUniqueName="[dim_ship_method]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[dim_ship_method].[Ship Method ID]" caption="Ship Method ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[dim_ship_method].[Ship Method ID].[All]" allUniqueName="[dim_ship_method].[Ship Method ID].[All]" dimensionUniqueName="[dim_ship_method]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[dim_vendor].[Business Entity ID]" caption="Business Entity ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[dim_vendor].[Business Entity ID].[All]" allUniqueName="[dim_vendor].[Business Entity ID].[All]" dimensionUniqueName="[dim_vendor]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[dim_vendor].[Jerarquía]" caption="Jerarquía" defaultMemberUniqueName="[dim_vendor].[Jerarquía].[All]" allUniqueName="[dim_vendor].[Jerarquía].[All]" dimensionUniqueName="[dim_vendor]" displayFolder="" count="2" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[dim_vendor].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[dim_vendor].[Name].[All]" allUniqueName="[dim_vendor].[Name].[All]" dimensionUniqueName="[dim_vendor]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Total Due]" caption="Total Due" measure="1" displayFolder="" measureGroup="Purchase Order Header" count="0" oneField="1">
-      <fieldsUsage count="1">
-        <fieldUsage x="0"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-  </cacheHierarchies>
-  <kpis count="0"/>
-  <dimensions count="4">
-    <dimension name="dim_employee" uniqueName="[dim_employee]" caption="dim_employee"/>
-    <dimension name="dim_ship_method" uniqueName="[dim_ship_method]" caption="dim_ship_method"/>
-    <dimension name="dim_vendor" uniqueName="[dim_vendor]" caption="dim_vendor"/>
-    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
-  </dimensions>
-  <measureGroups count="1">
-    <measureGroup name="Purchase Order Header" caption="Purchase Order Header"/>
-  </measureGroups>
-  <maps count="3">
-    <map measureGroup="0" dimension="0"/>
-    <map measureGroup="0" dimension="1"/>
-    <map measureGroup="0" dimension="2"/>
-  </maps>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Hugo Doradea" refreshedDate="44373.099563425923" backgroundQuery="1" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{C61F9162-62DE-4C5C-AFA1-CA6D16A03B11}">
-  <cacheSource type="external" connectionId="2"/>
-  <cacheFields count="2">
-    <cacheField name="[Measures].[Total Due]" caption="Total Due" numFmtId="0" hierarchy="9" level="32767"/>
-    <cacheField name="[dim_employee].[Jerarquía].[Gender]" caption="Gender" numFmtId="0" hierarchy="2" level="1">
-      <sharedItems count="2">
-        <s v="[dim_employee].[Jerarquía].[Gender].&amp;[F]" c="F"/>
-        <s v="[dim_employee].[Jerarquía].[Gender].&amp;[M]" c="M"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-  <cacheHierarchies count="10">
-    <cacheHierarchy uniqueName="[dim_employee].[Business Entity ID]" caption="Business Entity ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[dim_employee].[Business Entity ID].[All]" allUniqueName="[dim_employee].[Business Entity ID].[All]" dimensionUniqueName="[dim_employee]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[dim_employee].[Gender]" caption="Gender" attribute="1" defaultMemberUniqueName="[dim_employee].[Gender].[All]" allUniqueName="[dim_employee].[Gender].[All]" dimensionUniqueName="[dim_employee]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[dim_employee].[Jerarquía]" caption="Jerarquía" defaultMemberUniqueName="[dim_employee].[Jerarquía].[All]" allUniqueName="[dim_employee].[Jerarquía].[All]" dimensionUniqueName="[dim_employee]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[dim_ship_method].[Jerarquía]" caption="Jerarquía" defaultMemberUniqueName="[dim_ship_method].[Jerarquía].[All]" allUniqueName="[dim_ship_method].[Jerarquía].[All]" dimensionUniqueName="[dim_ship_method]" displayFolder="" count="2" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[dim_ship_method].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[dim_ship_method].[Name].[All]" allUniqueName="[dim_ship_method].[Name].[All]" dimensionUniqueName="[dim_ship_method]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[dim_ship_method].[Ship Method ID]" caption="Ship Method ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[dim_ship_method].[Ship Method ID].[All]" allUniqueName="[dim_ship_method].[Ship Method ID].[All]" dimensionUniqueName="[dim_ship_method]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[dim_vendor].[Business Entity ID]" caption="Business Entity ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[dim_vendor].[Business Entity ID].[All]" allUniqueName="[dim_vendor].[Business Entity ID].[All]" dimensionUniqueName="[dim_vendor]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[dim_vendor].[Jerarquía]" caption="Jerarquía" defaultMemberUniqueName="[dim_vendor].[Jerarquía].[All]" allUniqueName="[dim_vendor].[Jerarquía].[All]" dimensionUniqueName="[dim_vendor]" displayFolder="" count="2" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[dim_vendor].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[dim_vendor].[Name].[All]" allUniqueName="[dim_vendor].[Name].[All]" dimensionUniqueName="[dim_vendor]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Total Due]" caption="Total Due" measure="1" displayFolder="" measureGroup="Purchase Order Header" count="0" oneField="1">
-      <fieldsUsage count="1">
-        <fieldUsage x="0"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-  </cacheHierarchies>
-  <kpis count="0"/>
-  <dimensions count="4">
-    <dimension name="dim_employee" uniqueName="[dim_employee]" caption="dim_employee"/>
-    <dimension name="dim_ship_method" uniqueName="[dim_ship_method]" caption="dim_ship_method"/>
-    <dimension name="dim_vendor" uniqueName="[dim_vendor]" caption="dim_vendor"/>
-    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
-  </dimensions>
-  <measureGroups count="1">
-    <measureGroup name="Purchase Order Header" caption="Purchase Order Header"/>
-  </measureGroups>
-  <maps count="3">
-    <map measureGroup="0" dimension="0"/>
-    <map measureGroup="0" dimension="1"/>
-    <map measureGroup="0" dimension="2"/>
-  </maps>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6D50EBCC-F511-411F-A46A-6D57527DB10B}" name="table_compra_genero" cacheId="151" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6D50EBCC-F511-411F-A46A-6D57527DB10B}" name="table_compra_genero" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
   <location ref="E44:F47" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -4648,19 +4924,43 @@
     <dataField fld="0" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="3">
+    <format dxfId="1">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
-  <chartFormats count="1">
+  <chartFormats count="3">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -4694,7 +4994,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8A11F8B6-4592-4AED-87E3-DEB040094AA0}" name="table_compra_embargo" cacheId="142" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8A11F8B6-4592-4AED-87E3-DEB040094AA0}" name="table_compra_embargo" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
   <location ref="E26:F32" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -4738,19 +5038,79 @@
     <dataField fld="0" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="1">
+    <format dxfId="3">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="0">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
-  <chartFormats count="1">
+  <chartFormats count="6">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
           </reference>
         </references>
       </pivotArea>
@@ -4784,7 +5144,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{08B014A6-9999-41AB-8B7D-66A7E2FB2E2F}" name="table_compra_proveedor" cacheId="122" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{08B014A6-9999-41AB-8B7D-66A7E2FB2E2F}" name="table_compra_proveedor" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
   <location ref="B2:C89" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -5496,7 +5856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F8FFDB4-A903-4A3C-95A6-2449B72906CA}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -5509,10 +5869,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6003EA33-5B83-4A18-982B-C8DDFC6F68EB}">
-  <dimension ref="B2:K89"/>
+  <dimension ref="B2:K207"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E45" sqref="E45:F45"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5544,7 +5904,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="4">
-        <v>28502.091799999998</v>
+        <v>28502.091800000002</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -5594,7 +5954,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="4">
-        <v>30229.374800000005</v>
+        <v>30229.374800000001</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -5604,7 +5964,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="4">
-        <v>25060.0429</v>
+        <v>25060.042899999997</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -5615,7 +5975,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="4">
-        <v>79384.768000000011</v>
+        <v>79384.767999999996</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -5637,7 +5997,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="4">
-        <v>1952375.2986000001</v>
+        <v>1952375.2985999999</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -5681,7 +6041,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="4">
-        <v>8497.798499999999</v>
+        <v>8497.7985000000008</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -5703,7 +6063,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="4">
-        <v>561550.09519999987</v>
+        <v>561550.09519999998</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -5736,7 +6096,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="4">
-        <v>324301.47960000002</v>
+        <v>324301.47959999996</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -5791,7 +6151,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="4">
-        <v>3378.1736999999989</v>
+        <v>3378.1736999999998</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="1" t="s">
@@ -5807,7 +6167,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="4">
-        <v>22960.072400000005</v>
+        <v>22960.072399999997</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="2" t="s">
@@ -5823,7 +6183,7 @@
         <v>26</v>
       </c>
       <c r="C28" s="4">
-        <v>2472770.0523000006</v>
+        <v>2472770.0523000001</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="2" t="s">
@@ -5839,7 +6199,7 @@
         <v>27</v>
       </c>
       <c r="C29" s="4">
-        <v>31499.814100000003</v>
+        <v>31499.814099999996</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="2" t="s">
@@ -5855,7 +6215,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="4">
-        <v>1315488.5502000002</v>
+        <v>1315488.5501999999</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="2" t="s">
@@ -5871,7 +6231,7 @@
         <v>29</v>
       </c>
       <c r="C31" s="4">
-        <v>2154773.3718000003</v>
+        <v>2154773.3717999998</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="2" t="s">
@@ -5903,7 +6263,7 @@
         <v>31</v>
       </c>
       <c r="C33" s="4">
-        <v>71924.478900000016</v>
+        <v>71924.478900000002</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -5925,7 +6285,7 @@
         <v>33</v>
       </c>
       <c r="C35" s="4">
-        <v>2304231.5536000002</v>
+        <v>2304231.5535999998</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -5958,7 +6318,7 @@
         <v>36</v>
       </c>
       <c r="C38" s="4">
-        <v>25633.635299999998</v>
+        <v>25633.635300000002</v>
       </c>
       <c r="D38" s="3"/>
       <c r="H38"/>
@@ -5978,7 +6338,7 @@
         <v>38</v>
       </c>
       <c r="C40" s="4">
-        <v>2472770.0523000006</v>
+        <v>2472770.0523000001</v>
       </c>
       <c r="D40" s="3"/>
       <c r="H40"/>
@@ -5988,7 +6348,7 @@
         <v>39</v>
       </c>
       <c r="C41" s="4">
-        <v>401930.90310000005</v>
+        <v>401930.9031</v>
       </c>
       <c r="D41" s="3"/>
       <c r="H41"/>
@@ -6009,7 +6369,7 @@
         <v>41</v>
       </c>
       <c r="C43" s="4">
-        <v>1268930.0360999997</v>
+        <v>1268930.0360999999</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43"/>
@@ -6020,7 +6380,7 @@
         <v>42</v>
       </c>
       <c r="C44" s="4">
-        <v>1952375.2985999994</v>
+        <v>1952375.2985999999</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="1" t="s">
@@ -6036,7 +6396,7 @@
         <v>43</v>
       </c>
       <c r="C45" s="4">
-        <v>27308.607400000004</v>
+        <v>27308.607400000001</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="2" t="s">
@@ -6068,7 +6428,7 @@
         <v>45</v>
       </c>
       <c r="C47" s="4">
-        <v>8061.1008000000002</v>
+        <v>8061.1007999999993</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="2" t="s">
@@ -6084,7 +6444,7 @@
         <v>46</v>
       </c>
       <c r="C48" s="4">
-        <v>1589172.9591000003</v>
+        <v>1589172.9591000001</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
@@ -6095,7 +6455,7 @@
         <v>47</v>
       </c>
       <c r="C49" s="4">
-        <v>209264.42909999998</v>
+        <v>209264.42910000001</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
@@ -6139,7 +6499,7 @@
         <v>51</v>
       </c>
       <c r="C53" s="4">
-        <v>321870.17490000004</v>
+        <v>321870.17489999998</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
@@ -6150,7 +6510,7 @@
         <v>52</v>
       </c>
       <c r="C54" s="4">
-        <v>27177.800499999998</v>
+        <v>27177.800500000001</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
@@ -6161,7 +6521,7 @@
         <v>53</v>
       </c>
       <c r="C55" s="4">
-        <v>5412.5649999999987</v>
+        <v>5412.5649999999996</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
@@ -6194,7 +6554,7 @@
         <v>56</v>
       </c>
       <c r="C58" s="4">
-        <v>7328.72</v>
+        <v>7328.7199999999993</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
@@ -6205,7 +6565,7 @@
         <v>57</v>
       </c>
       <c r="C59" s="4">
-        <v>2424284.3650000002</v>
+        <v>2424284.3649999998</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
@@ -6227,7 +6587,7 @@
         <v>59</v>
       </c>
       <c r="C61" s="4">
-        <v>39754.446499999991</v>
+        <v>39754.446499999998</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
@@ -6238,7 +6598,7 @@
         <v>60</v>
       </c>
       <c r="C62" s="4">
-        <v>25513.899999999998</v>
+        <v>25513.899999999994</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -6293,7 +6653,7 @@
         <v>65</v>
       </c>
       <c r="C67" s="4">
-        <v>3379946.3215000005</v>
+        <v>3379946.3215000001</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
@@ -6315,7 +6675,7 @@
         <v>67</v>
       </c>
       <c r="C69" s="4">
-        <v>23635.058400000005</v>
+        <v>23635.058400000002</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
@@ -6359,7 +6719,7 @@
         <v>71</v>
       </c>
       <c r="C73" s="4">
-        <v>2675889.2159999991</v>
+        <v>2675889.2159999995</v>
       </c>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
@@ -6414,7 +6774,7 @@
         <v>76</v>
       </c>
       <c r="C78" s="4">
-        <v>91088.374599999996</v>
+        <v>91088.37460000001</v>
       </c>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
@@ -6425,7 +6785,7 @@
         <v>77</v>
       </c>
       <c r="C79" s="4">
-        <v>577793.36319999991</v>
+        <v>577793.36320000002</v>
       </c>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
@@ -6447,7 +6807,7 @@
         <v>79</v>
       </c>
       <c r="C81" s="4">
-        <v>52176.445000000007</v>
+        <v>52176.445</v>
       </c>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
@@ -6458,7 +6818,7 @@
         <v>80</v>
       </c>
       <c r="C82" s="4">
-        <v>2052173.6244000001</v>
+        <v>2052173.6244000003</v>
       </c>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
@@ -6469,7 +6829,7 @@
         <v>81</v>
       </c>
       <c r="C83" s="4">
-        <v>2777684.9109999998</v>
+        <v>2777684.9110000003</v>
       </c>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
@@ -6513,7 +6873,7 @@
         <v>85</v>
       </c>
       <c r="C87" s="4">
-        <v>8025.5997000000007</v>
+        <v>8025.5996999999988</v>
       </c>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
@@ -6535,11 +6895,365 @@
         <v>87</v>
       </c>
       <c r="C89" s="4">
-        <v>70479332.638300017</v>
+        <v>70479332.638300046</v>
       </c>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
       <c r="H89"/>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C90"/>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C91"/>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C92"/>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C93"/>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C94"/>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C95"/>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C96"/>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C97"/>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C98"/>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C99"/>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C100"/>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C101"/>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C102"/>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C103"/>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C104"/>
+    </row>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C105"/>
+    </row>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C106"/>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C107"/>
+    </row>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C108"/>
+    </row>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C109"/>
+    </row>
+    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C110"/>
+    </row>
+    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C111"/>
+    </row>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C112"/>
+    </row>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C113"/>
+    </row>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C114"/>
+    </row>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C115"/>
+    </row>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C116"/>
+    </row>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C117"/>
+    </row>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C118"/>
+    </row>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C119"/>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C120"/>
+    </row>
+    <row r="121" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C121"/>
+    </row>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C122"/>
+    </row>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C123"/>
+    </row>
+    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C124"/>
+    </row>
+    <row r="125" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C125"/>
+    </row>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C126"/>
+    </row>
+    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C127"/>
+    </row>
+    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C128"/>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C129"/>
+    </row>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C130"/>
+    </row>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C131"/>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C132"/>
+    </row>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C133"/>
+    </row>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C134"/>
+    </row>
+    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C135"/>
+    </row>
+    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C136"/>
+    </row>
+    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C137"/>
+    </row>
+    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C138"/>
+    </row>
+    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C139"/>
+    </row>
+    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C140"/>
+    </row>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C141"/>
+    </row>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C142"/>
+    </row>
+    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C143"/>
+    </row>
+    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C144"/>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C145"/>
+    </row>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C146"/>
+    </row>
+    <row r="147" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C147"/>
+    </row>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C148"/>
+    </row>
+    <row r="149" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C149"/>
+    </row>
+    <row r="150" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C150"/>
+    </row>
+    <row r="151" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C151"/>
+    </row>
+    <row r="152" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C152"/>
+    </row>
+    <row r="153" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C153"/>
+    </row>
+    <row r="154" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C154"/>
+    </row>
+    <row r="155" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C155"/>
+    </row>
+    <row r="156" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C156"/>
+    </row>
+    <row r="157" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C157"/>
+    </row>
+    <row r="158" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C158"/>
+    </row>
+    <row r="159" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C159"/>
+    </row>
+    <row r="160" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C160"/>
+    </row>
+    <row r="161" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C161"/>
+    </row>
+    <row r="162" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C162"/>
+    </row>
+    <row r="163" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C163"/>
+    </row>
+    <row r="164" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C164"/>
+    </row>
+    <row r="165" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C165"/>
+    </row>
+    <row r="166" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C166"/>
+    </row>
+    <row r="167" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C167"/>
+    </row>
+    <row r="168" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C168"/>
+    </row>
+    <row r="169" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C169"/>
+    </row>
+    <row r="170" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C170"/>
+    </row>
+    <row r="171" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C171"/>
+    </row>
+    <row r="172" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C172"/>
+    </row>
+    <row r="173" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C173"/>
+    </row>
+    <row r="174" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C174"/>
+    </row>
+    <row r="175" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C175"/>
+    </row>
+    <row r="176" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C176"/>
+    </row>
+    <row r="177" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C177"/>
+    </row>
+    <row r="178" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C178"/>
+    </row>
+    <row r="179" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C179"/>
+    </row>
+    <row r="180" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C180"/>
+    </row>
+    <row r="181" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C181"/>
+    </row>
+    <row r="182" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C182"/>
+    </row>
+    <row r="183" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C183"/>
+    </row>
+    <row r="184" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C184"/>
+    </row>
+    <row r="185" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C185"/>
+    </row>
+    <row r="186" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C186"/>
+    </row>
+    <row r="187" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C187"/>
+    </row>
+    <row r="188" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C188"/>
+    </row>
+    <row r="189" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C189"/>
+    </row>
+    <row r="190" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C190"/>
+    </row>
+    <row r="191" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C191"/>
+    </row>
+    <row r="192" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C192"/>
+    </row>
+    <row r="193" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C193"/>
+    </row>
+    <row r="194" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C194"/>
+    </row>
+    <row r="195" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C195"/>
+    </row>
+    <row r="196" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C196"/>
+    </row>
+    <row r="197" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C197"/>
+    </row>
+    <row r="198" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C198"/>
+    </row>
+    <row r="199" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C199"/>
+    </row>
+    <row r="200" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C200"/>
+    </row>
+    <row r="201" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C201"/>
+    </row>
+    <row r="202" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C202"/>
+    </row>
+    <row r="203" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C203"/>
+    </row>
+    <row r="204" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C204"/>
+    </row>
+    <row r="205" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C205"/>
+    </row>
+    <row r="206" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C206"/>
+    </row>
+    <row r="207" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C207"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>